<commit_message>
Initial commit of main script
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96325B69-C69A-484B-8799-A430DDEAA61F}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8218C2D-182D-4A58-B506-C459230F6FBF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORSCHUNGSFRAGE" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="132">
   <si>
     <t>Forschungsfrage:</t>
   </si>
@@ -168,9 +168,6 @@
     <t>output</t>
   </si>
   <si>
-    <t>transkripte</t>
-  </si>
-  <si>
     <t>definition</t>
   </si>
   <si>
@@ -394,6 +391,39 @@
   </si>
   <si>
     <t>Diese Kategorie umfasst alle zukunftsgerichteten Aussagen zur strategischen Entwicklung und Ausrichtung der Forschung an Hochschulen. Dies beinhaltet sowohl konkrete Entwicklungspläne und Zielsetzungen als auch Visionen und Wünsche für die zukünftige Forschungslandschaft. Dabei werden sowohl institutionelle Strategien als auch individuelle Perspektiven sowie die damit verbundenen Chancen und Herausforderungen berücksichtigt.</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Label für erstes Partikel des Dateinamens, getrennt mit "_"</t>
+  </si>
+  <si>
+    <t>Label für zweites Partikel des Dateinamens, getrennt mit "_"</t>
+  </si>
+  <si>
+    <t>Höhere Temperatur führt zu mehr Varianz der Antwort</t>
+  </si>
+  <si>
+    <t>Zeichenlänge des Textsegments</t>
+  </si>
+  <si>
+    <t>Überlappungsbereich (10%)</t>
+  </si>
+  <si>
+    <t>Eingabedokumente</t>
+  </si>
+  <si>
+    <t>Ausgabe</t>
+  </si>
+  <si>
+    <t>OpenAI Modell</t>
+  </si>
+  <si>
+    <t>Name des ersten KI-Coders</t>
+  </si>
+  <si>
+    <t>Name des zweiten KI-Coders</t>
   </si>
 </sst>
 </file>
@@ -673,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -764,6 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1061,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1076,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83632032-027F-4E92-9508-DC0162C427A9}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -1107,11 +1138,11 @@
         <v>11</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1119,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
@@ -1131,13 +1162,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,13 +1176,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1159,13 +1190,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1173,13 +1204,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1187,11 +1218,11 @@
         <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,13 +1230,13 @@
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,13 +1244,13 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,13 +1258,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,13 +1272,13 @@
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1255,13 +1286,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,13 +1300,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,13 +1314,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,13 +1328,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,33 +1342,33 @@
         <v>13</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6" t="s">
@@ -1346,114 +1377,114 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -1461,11 +1492,11 @@
         <v>15</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,13 +1504,13 @@
         <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1487,13 +1518,13 @@
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,13 +1532,13 @@
         <v>15</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,13 +1546,13 @@
         <v>15</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1529,13 +1560,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,13 +1574,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1557,13 +1588,13 @@
         <v>15</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,13 +1602,13 @@
         <v>15</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,13 +1616,13 @@
         <v>15</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -1599,11 +1630,11 @@
         <v>16</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1611,13 +1642,13 @@
         <v>16</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1625,13 +1656,13 @@
         <v>16</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1639,13 +1670,13 @@
         <v>16</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1653,13 +1684,13 @@
         <v>16</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,13 +1698,13 @@
         <v>16</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1681,13 +1712,13 @@
         <v>16</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,13 +1726,13 @@
         <v>16</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1709,13 +1740,13 @@
         <v>16</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,13 +1754,13 @@
         <v>16</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -1737,11 +1768,11 @@
         <v>17</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1749,7 +1780,7 @@
         <v>17</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="6" t="s">
@@ -1761,13 +1792,13 @@
         <v>17</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,13 +1806,13 @@
         <v>17</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,13 +1820,13 @@
         <v>17</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,13 +1834,13 @@
         <v>17</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -1817,11 +1848,11 @@
         <v>19</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,7 +1860,7 @@
         <v>19</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="6" t="s">
@@ -1841,13 +1872,13 @@
         <v>19</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,13 +1886,13 @@
         <v>19</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,13 +1900,13 @@
         <v>19</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1883,13 +1914,13 @@
         <v>19</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2026,10 +2057,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0733A825-A3F8-434F-8803-3EA195D106E6}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,9 +2069,10 @@
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
@@ -2053,8 +2085,9 @@
       <c r="D1" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
@@ -2063,18 +2096,24 @@
       <c r="D2" s="33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -2083,8 +2122,11 @@
       <c r="D4" s="27" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
@@ -2093,8 +2135,11 @@
       <c r="D5" s="26">
         <v>800</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
@@ -2103,8 +2148,11 @@
       <c r="D6" s="26">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>31</v>
       </c>
@@ -2115,8 +2163,11 @@
       <c r="D7" s="26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
@@ -2127,8 +2178,11 @@
       <c r="D8" s="26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>36</v>
       </c>
@@ -2141,8 +2195,11 @@
       <c r="D9" s="26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>36</v>
       </c>
@@ -2155,8 +2212,11 @@
       <c r="D10" s="26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -2169,8 +2229,11 @@
       <c r="D11" s="26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
@@ -2182,6 +2245,9 @@
       </c>
       <c r="D12" s="28" t="s">
         <v>44</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add exclusion criteria for relevance check
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{152591A0-821D-4572-950B-59A1320DAC6E}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66AA438B-CA98-4C75-9A68-EB1F8AE3AAE6}"/>
   <bookViews>
-    <workbookView xWindow="-4358" yWindow="8002" windowWidth="21796" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORSCHUNGSFRAGE" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="179">
   <si>
     <t>Forschungsfrage:</t>
   </si>
@@ -553,6 +553,18 @@
   </si>
   <si>
     <t>Der Name des verwendeten Modells, Standard: "gpt-4o-mini", "mistral-small"</t>
+  </si>
+  <si>
+    <t>Ausschlussregeln</t>
+  </si>
+  <si>
+    <t>Literaturverzeichnisse und Referenzlisten</t>
+  </si>
+  <si>
+    <t>Tabellarische Datenaufstellungen</t>
+  </si>
+  <si>
+    <t>Methodische Infoboxen</t>
   </si>
 </sst>
 </file>
@@ -2051,125 +2063,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31726682-FB53-460D-AA9E-961E482F9726}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.140625" customWidth="1"/>
-    <col min="2" max="2" width="67.140625" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="21"/>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="21"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="21"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="21"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="21"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="21"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="21"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="21"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="21"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="21"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2180,7 +2223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0733A825-A3F8-434F-8803-3EA195D106E6}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add third doc attribute
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3389A29-1E59-4707-A6B8-87262284E8C6}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B22B61C4-2692-453A-9480-661C31DA7CDA}"/>
   <bookViews>
-    <workbookView xWindow="-3750" yWindow="8002" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORSCHUNGSFRAGE" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="187">
   <si>
     <t>Forschungsfrage:</t>
   </si>
@@ -583,6 +583,12 @@
   </si>
   <si>
     <t>full (volle induktive Analyse) - abductive (nur Subkategorien entwickeln) - deductive (nur deduktiv)</t>
+  </si>
+  <si>
+    <t>attribut3</t>
+  </si>
+  <si>
+    <t>Frei lassen, wenn nicht benötigt</t>
   </si>
 </sst>
 </file>
@@ -2242,10 +2248,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0733A825-A3F8-434F-8803-3EA195D106E6}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,19 +2429,15 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>39</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="31" t="s">
-        <v>131</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2446,13 +2448,13 @@
         <v>37</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,16 +2462,16 @@
         <v>36</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2480,28 +2482,30 @@
         <v>42</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2509,14 +2513,14 @@
         <v>135</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="24">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2524,14 +2528,14 @@
         <v>135</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="24" t="s">
-        <v>141</v>
+      <c r="D19" s="24">
+        <v>2</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2539,14 +2543,14 @@
         <v>135</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="24">
-        <v>2</v>
+      <c r="D20" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,14 +2558,14 @@
         <v>135</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="24">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2569,14 +2573,14 @@
         <v>135</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="24">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2584,16 +2588,14 @@
         <v>135</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="24">
+        <v>3</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,7 +2606,7 @@
         <v>149</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>151</v>
@@ -2621,7 +2623,7 @@
         <v>149</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>151</v>
@@ -2638,7 +2640,7 @@
         <v>149</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>151</v>
@@ -2655,7 +2657,7 @@
         <v>149</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>151</v>
@@ -2672,7 +2674,7 @@
         <v>149</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D28" s="24" t="s">
         <v>151</v>
@@ -2686,16 +2688,16 @@
         <v>135</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2706,13 +2708,13 @@
         <v>158</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2723,16 +2725,16 @@
         <v>158</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>135</v>
       </c>
@@ -2740,12 +2742,29 @@
         <v>158</v>
       </c>
       <c r="C32" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D33" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E33" s="31" t="s">
         <v>170</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add manual review and majority voting
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1411A42-6658-4317-B976-0428EB88F23A}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEFB3376-2109-4801-92CC-B703BFCD2034}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORSCHUNGSFRAGE" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="189">
   <si>
     <t>Forschungsfrage:</t>
   </si>
@@ -540,9 +540,6 @@
     <t>Unterstützt "OpenAI" und "Mistral"</t>
   </si>
   <si>
-    <t>Der Name des verwendeten Modells, Standard: "gpt-4o-mini", "mistral-small"</t>
-  </si>
-  <si>
     <t>Ausschlussregeln</t>
   </si>
   <si>
@@ -585,10 +582,19 @@
     <t>Eine Kennung für den ersten Coder, frei wählbarer Name</t>
   </si>
   <si>
-    <t>Einstellung für den zweiten Coder, frei wählbarer Name</t>
-  </si>
-  <si>
     <t>gpt-4.1-mini</t>
+  </si>
+  <si>
+    <t>REVIEW_MODE</t>
+  </si>
+  <si>
+    <t>consensus</t>
+  </si>
+  <si>
+    <t>consensus' (Default), 'manual', oder 'majority' - hier festlegen, wie Unstimmigkeiten zwischen Kodierern aufgelöst werden sollen</t>
+  </si>
+  <si>
+    <t>Der Name des verwendeten Modells, Standard: "gpt-4o-mini" oder "gpt-4.1-mini", "mistral-small"</t>
   </si>
 </sst>
 </file>
@@ -868,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -953,6 +959,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1267,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83632032-027F-4E92-9508-DC0162C427A9}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2122,7 +2131,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2133,7 +2142,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2144,7 +2153,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2248,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0733A825-A3F8-434F-8803-3EA195D106E6}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,10 +2309,10 @@
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2313,7 +2322,7 @@
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E4" s="31" t="s">
         <v>121</v>
@@ -2373,43 +2382,41 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>179</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>31</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>127</v>
+        <v>186</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2417,14 +2424,14 @@
         <v>30</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2432,29 +2439,27 @@
         <v>30</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>181</v>
+        <v>33</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="E13" s="31" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>38</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="31" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2465,13 +2470,13 @@
         <v>36</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>184</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2479,16 +2484,16 @@
         <v>35</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2499,28 +2504,30 @@
         <v>41</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>131</v>
+        <v>35</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24">
-        <v>15</v>
+        <v>41</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2528,14 +2535,14 @@
         <v>131</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="24">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2543,14 +2550,14 @@
         <v>131</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="24" t="s">
-        <v>137</v>
+      <c r="D20" s="24">
+        <v>2</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2558,14 +2565,14 @@
         <v>131</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="24">
-        <v>2</v>
+      <c r="D21" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2573,14 +2580,14 @@
         <v>131</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="24">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2588,14 +2595,14 @@
         <v>131</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="24">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,16 +2610,14 @@
         <v>131</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="24">
+        <v>3</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2623,7 +2628,7 @@
         <v>145</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>147</v>
@@ -2640,7 +2645,7 @@
         <v>145</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>147</v>
@@ -2657,7 +2662,7 @@
         <v>145</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>147</v>
@@ -2674,7 +2679,7 @@
         <v>145</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D28" s="24" t="s">
         <v>147</v>
@@ -2691,7 +2696,7 @@
         <v>145</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>147</v>
@@ -2705,16 +2710,16 @@
         <v>131</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2725,13 +2730,13 @@
         <v>154</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2742,16 +2747,16 @@
         <v>154</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>131</v>
       </c>
@@ -2759,12 +2764,29 @@
         <v>154</v>
       </c>
       <c r="C33" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D34" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E34" s="31" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix for parallelization in v0.9.15
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD559E3D-866C-4C88-ABD7-D71B5790616A}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA56FA56-CD76-457D-9DF2-F7250202AD2C}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORSCHUNGSFRAGE" sheetId="1" r:id="rId1"/>
@@ -615,12 +615,6 @@
     <t>MULTIPLE_CODING_THRESHOLD</t>
   </si>
   <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>Relevanzschwelle für die Entscheidung ob ein Segment mehr als eine Hauptkategorie zugewiesen werden soll. Default '0.7'</t>
-  </si>
-  <si>
     <t>full (volle induktive Analyse) - abductive (nur Subkategorien entwickeln) - deductive (nur deduktiv) - grounded (Hauptkategorien zum Schluss bilden)</t>
   </si>
   <si>
@@ -628,6 +622,12 @@
   </si>
   <si>
     <t>Mehrfachkodierung (Hauptkategorien) eines Segments erlauben (Default 'true')</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>Relevanzschwelle für die Entscheidung ob ein Segment mehr als eine Hauptkategorie zugewiesen werden soll. Default '0.8'</t>
   </si>
 </sst>
 </file>
@@ -2155,7 +2155,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,7 +2282,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>96</v>
@@ -2298,7 +2298,7 @@
         <v>68</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2308,10 +2308,10 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="25" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2324,7 +2324,7 @@
         <v>98</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Phase 7: I/O Module - Document Processing and Escape Handler
Extracted document reading and escape key handling from QCA_Utils.py.

- DocumentReader: TXT, DOCX, PDF support with text extraction
- EscapeHandler: Graceful shutdown on ESC with intermediate export
- Total: ~730 lines, full backward compatibility

🐻 Generated with Crush
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{4C215F05-F5BD-4B4A-9F1D-DA979642D93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6EC56BC-7496-4C4F-BD66-090F6ECC3591}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4F95FC8-2993-4BA3-A82D-446773B864AE}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORSCHUNGSFRAGE" sheetId="1" r:id="rId1"/>
@@ -336,9 +336,6 @@
     <t>Eine Kennung für den ersten Coder, frei wählbarer Name</t>
   </si>
   <si>
-    <t>gpt-4.1-mini</t>
-  </si>
-  <si>
     <t>REVIEW_MODE</t>
   </si>
   <si>
@@ -640,6 +637,9 @@
   </si>
   <si>
     <t>Schwellenwert für Fuzzy-Text-Matching</t>
+  </si>
+  <si>
+    <t>gpt-5-nano</t>
   </si>
 </sst>
 </file>
@@ -1336,6 +1336,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="5">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{34D127E0-B7FD-47A2-A2F5-EBC62D3AF3F9}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
@@ -1344,21 +1371,21 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="108.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="108.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
     </row>
   </sheetData>
@@ -1374,15 +1401,15 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.73046875" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="24.265625" customWidth="1"/>
-    <col min="4" max="4" width="103.265625" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="103.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
@@ -1396,89 +1423,89 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="D4" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="22" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="22" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="22" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>37</v>
@@ -1487,12 +1514,12 @@
         <v>26</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>37</v>
@@ -1501,12 +1528,12 @@
         <v>31</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>37</v>
@@ -1515,12 +1542,12 @@
         <v>38</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>37</v>
@@ -1529,483 +1556,483 @@
         <v>39</v>
       </c>
       <c r="D11" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="20" t="s">
-        <v>122</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="22" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="21" t="s">
+      <c r="D14" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="22" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="D15" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="22" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="D16" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="22" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="20" t="s">
-        <v>132</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="21"/>
       <c r="D17" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="D18" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="22" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="21" t="s">
+      <c r="D19" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="22" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="D20" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="22" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="21" t="s">
+      <c r="D21" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D21" s="22" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="20" t="s">
-        <v>142</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="21" t="s">
+      <c r="D23" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D23" s="22" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="21" t="s">
+      <c r="D24" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="D24" s="22" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="21" t="s">
+      <c r="D25" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="D25" s="22" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="21" t="s">
+      <c r="D26" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="22" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="20" t="s">
-        <v>152</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="21"/>
       <c r="D27" s="22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="21" t="s">
+      <c r="D28" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="22" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="21" t="s">
+      <c r="D29" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="D29" s="22" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="21" t="s">
+      <c r="D30" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="D30" s="22" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="21" t="s">
+      <c r="D31" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="D31" s="22" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="20" t="s">
-        <v>162</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="D33" s="22" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="21" t="s">
+      <c r="D34" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="22" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="21" t="s">
+      <c r="D35" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="22" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B36" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="D36" s="22" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="20" t="s">
-        <v>172</v>
       </c>
       <c r="B37" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="22" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A39" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="21" t="s">
+      <c r="D39" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="D39" s="22" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="21" t="s">
+      <c r="D40" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="D40" s="22" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C41" s="21" t="s">
+      <c r="D41" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="D41" s="22" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" s="20" t="s">
-        <v>181</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" s="21" t="s">
+      <c r="D43" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="D43" s="22" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A44" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="21" t="s">
+      <c r="D44" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="D44" s="22" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A45" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="21" t="s">
+      <c r="D45" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D45" s="22" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="21" t="s">
+      <c r="D46" s="22" t="s">
         <v>189</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2021,14 +2048,14 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.1328125" customWidth="1"/>
-    <col min="2" max="2" width="53.265625" customWidth="1"/>
-    <col min="3" max="3" width="52.73046875" customWidth="1"/>
+    <col min="1" max="1" width="64.109375" customWidth="1"/>
+    <col min="2" max="2" width="53.21875" customWidth="1"/>
+    <col min="3" max="3" width="52.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2039,7 +2066,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -2050,7 +2077,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -2061,7 +2088,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -2072,96 +2099,96 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -2175,20 +2202,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0733A825-A3F8-434F-8803-3EA195D106E6}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.1328125" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="4" width="23.59765625" customWidth="1"/>
-    <col min="5" max="5" width="55.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="55.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>11</v>
       </c>
@@ -2205,7 +2232,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>87</v>
       </c>
@@ -2218,20 +2245,20 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="25" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -2244,7 +2271,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -2257,7 +2284,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2270,7 +2297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -2283,7 +2310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
@@ -2293,25 +2320,25 @@
         <v>5</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2319,23 +2346,23 @@
         <v>67</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>96</v>
       </c>
@@ -2345,23 +2372,23 @@
         <v>97</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2403,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -2391,7 +2418,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2404,9 +2431,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2414,23 +2441,23 @@
         <v>67</v>
       </c>
       <c r="E17" s="28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="30" t="s">
-        <v>202</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
@@ -2447,7 +2474,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
@@ -2464,7 +2491,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -2481,7 +2508,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
@@ -2498,7 +2525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
@@ -2513,7 +2540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>51</v>
       </c>
@@ -2528,7 +2555,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
@@ -2543,7 +2570,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
@@ -2558,7 +2585,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
@@ -2573,7 +2600,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
@@ -2588,7 +2615,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
@@ -2605,7 +2632,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>51</v>
       </c>
@@ -2622,7 +2649,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>51</v>
       </c>
@@ -2639,7 +2666,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>51</v>
       </c>
@@ -2656,7 +2683,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>51</v>
       </c>
@@ -2673,7 +2700,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>51</v>
       </c>
@@ -2690,7 +2717,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="30" t="s">
         <v>51</v>
       </c>
@@ -2707,7 +2734,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
         <v>51</v>
       </c>
@@ -2724,7 +2751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
         <v>51</v>
       </c>
@@ -2741,7 +2768,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="33" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
refactor: complete removal of QCA_Utils.py - all functions migrated to modular structure
- Extracted validators to utils/validators.py (category and selection validation)
- Extracted dialog helpers to utils/dialog_helpers.py (window setup, result formatting)
- Extracted impact analysis to utils/impact_analysis.py (coding impact analysis, reporting)
- Extracted DocumentToPDFConverter to utils/export/converters.py
- Updated all imports in analysis_manager.py, results_exporter.py, manual_coding.py, main.py
- Deleted legacy QCA_Utils.py (235 lines) - now 100% refactored
- All 5,836 lines of original utilities are now organized in focused modules
- All imports verified and syntax checked
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4F95FC8-2993-4BA3-A82D-446773B864AE}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93F4F843-597A-44A5-815E-1F8785F37A9C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,7 +639,7 @@
     <t>Schwellenwert für Fuzzy-Text-Matching</t>
   </si>
   <si>
-    <t>gpt-5-nano</t>
+    <t>gpt-40-mini</t>
   </si>
 </sst>
 </file>
@@ -1354,6 +1354,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -2203,7 +2206,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="A9:D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix: add float type conversion for threshold and confidence comparisons
- Convert MULTIPLE_CODING_THRESHOLD to float in RelevanceChecker.__init__
- Convert confidence values to float before comparison in inductive_coding.py
- Prevents '>=' not supported between instances of 'float' and 'str' errors
- Ensures type safety when comparing config values that may come as strings from Excel
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93F4F843-597A-44A5-815E-1F8785F37A9C}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5805D50F-7718-4761-B71B-30DDD8429031}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,7 +639,7 @@
     <t>Schwellenwert für Fuzzy-Text-Matching</t>
   </si>
   <si>
-    <t>gpt-40-mini</t>
+    <t>gpt-4o-mini</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2206,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
chore: release version 0.10.1 with paraphrase context and bugfixes
- Implement paraphrase-based batch context for improved coding comprehension
- Add "Kontext_verwendet" column to Excel export
- Fix RelevanceChecker justification field duplication
- Fix inductive coding mode datetime import error
- Fix CategoryDefinition None definition handling
- Resolve export table begründung logic duplication
- Remove 1089 lines of dead/duplicate code
- Ensure batches contain segments from single document only
- Update version numbers to 0.10.1 across all files

🐻 Generated with Crush

Co-Authored-By: Crush <crush@charm.land>
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A5494A1-AEBC-404B-AD76-B1B0E5386A14}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8486AB42-E7C7-4785-B6DE-CFAE4EC94D1C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="203">
   <si>
     <t>Forschungsfrage:</t>
   </si>
@@ -606,12 +606,6 @@
     <t>MULTIPLE_CODING_THRESHOLD</t>
   </si>
   <si>
-    <t>full (volle induktive Analyse) - abductive (nur Subkategorien entwickeln) - deductive (nur deduktiv) - grounded (Hauptkategorien zum Schluss bilden)</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Mehrfachkodierung (Hauptkategorien) eines Segments erlauben (Default 'true')</t>
   </si>
   <si>
@@ -639,7 +633,10 @@
     <t>gpt-4o-mini</t>
   </si>
   <si>
-    <t>deductive</t>
+    <t>inductive</t>
+  </si>
+  <si>
+    <t>inductive (volle induktive Analyse) - abductive (nur Subkategorien entwickeln) - deductive (nur deduktiv) - grounded (Hauptkategorien zum Schluss bilden)</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2203,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2255,7 +2252,7 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>104</v>
@@ -2323,7 +2320,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2333,7 +2330,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="25" t="s">
-        <v>193</v>
+        <v>67</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>95</v>
@@ -2349,7 +2346,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2359,10 +2356,10 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2372,10 +2369,10 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2436,7 +2433,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2444,20 +2441,20 @@
         <v>67</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Version 0.10.2: QCA-AID-Explorer Refactoring - Modulare Architektur & JSON-Konfiguration
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01b812a4e606ac90/Projekte/Forschung/R-Projects/QCA-AID/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8486AB42-E7C7-4785-B6DE-CFAE4EC94D1C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{EF7502F4-0FAA-42F9-86ED-E898BDC33C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C72B315C-467D-4723-AC9A-01F0A022017C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,10 +633,10 @@
     <t>gpt-4o-mini</t>
   </si>
   <si>
-    <t>inductive</t>
-  </si>
-  <si>
     <t>inductive (volle induktive Analyse) - abductive (nur Subkategorien entwickeln) - deductive (nur deduktiv) - grounded (Hauptkategorien zum Schluss bilden)</t>
+  </si>
+  <si>
+    <t>deductive</t>
   </si>
 </sst>
 </file>
@@ -2203,7 +2203,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2369,10 +2369,10 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>201</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update project files and add QCA-AID webapp
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -1547,7 +1547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1585,14 +1585,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MODEL_PROVIDER</t>
+          <t>model_provider</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>OpenAI</t>
+          <t>openai</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1600,14 +1600,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MODEL_NAME</t>
+          <t>model_name</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>gpt-4o-mini</t>
+          <t>gpt-5-nano</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1615,7 +1615,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DATA_DIR</t>
+          <t>data_dir</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -1630,7 +1630,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OUTPUT_DIR</t>
+          <t>output_dir</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -1645,46 +1645,46 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CHUNK_SIZE</t>
+          <t>chunk_size</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CHUNK_OVERLAP</t>
+          <t>chunk_overlap</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BATCH_SIZE</t>
+          <t>batch_size</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CODE_WITH_CONTEXT</t>
+          <t>code_with_context</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -1697,7 +1697,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MULTIPLE_CODINGS</t>
+          <t>multiple_codings</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -1710,7 +1710,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MULTIPLE_CODING_THRESHOLD</t>
+          <t>multiple_coding_threshold</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1723,7 +1723,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ANALYSIS_MODE</t>
+          <t>analysis_mode</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1738,14 +1738,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>REVIEW_MODE</t>
+          <t>review_mode</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>consensus</t>
+          <t>auto</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -1753,7 +1753,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ATTRIBUTE_LABELS</t>
+          <t>attribute_labels</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1764,7 +1764,7 @@
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Hochschulprofil</t>
+          <t>Fall</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -1772,7 +1772,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ATTRIBUTE_LABELS</t>
+          <t>attribute_labels</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1783,7 +1783,7 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Akteur</t>
+          <t>Typ</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1791,463 +1791,129 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ATTRIBUTE_LABELS</t>
+          <t>coder_settings</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>attribut3</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+          <t>[0]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>temperature</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3</v>
+      </c>
       <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EXPORT_ANNOTATED_PDFS</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="n">
-        <v>1</v>
+          <t>coder_settings</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>coder_id</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>auto_1</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PDF_ANNOTATION_FUZZY_THRESHOLD</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
+          <t>coder_settings</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>temperature</t>
+        </is>
+      </c>
       <c r="D18" t="n">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CODER_SETTINGS</t>
+          <t>coder_settings</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[0]</t>
+          <t>[1]</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>temperature</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>0.3</v>
+          <t>coder_id</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>auto_2</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CODER_SETTINGS</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[0]</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>coder_id</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>auto_1</t>
-        </is>
+          <t>manual_coding_enabled</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CODER_SETTINGS</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>temperature</t>
-        </is>
-      </c>
+          <t>export_annotated_pdfs</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CODER_SETTINGS</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>coder_id</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>auto_2</t>
-        </is>
+          <t>pdf_annotation_fuzzy_threshold</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>0.85</v>
       </c>
       <c r="E22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>MIN_DEFINITION_WORDS</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>MIN_EXAMPLES</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>SIMILARITY_THRESHOLD</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0.7</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>MIN_SUBCATEGORIES</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>MAX_NAME_LENGTH</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>MIN_NAME_LENGTH</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>ENGLISH_WORDS</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>research</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>ENGLISH_WORDS</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>development</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>ENGLISH_WORDS</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>management</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>ENGLISH_WORDS</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>system</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>ENGLISH_WORDS</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>process</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>ENGLISH_WORDS</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>analysis</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>MESSAGES</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>short_definition</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Definition zu kurz (min. {min_words} Wörter)</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>MESSAGES</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>few_examples</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Zu wenige Beispiele (min. {min_examples})</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>MESSAGES</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>english_terms</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Name enthält englische Begriffe</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>VALIDATION</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>MESSAGES</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>name_length</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Name muss zwischen {min_len} und {max_len} Zeichen sein  </t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Release v0.11.1: Bugfixes und automatisches Config-Update
Bugfixes:
- Setup.bat erstellt Desktop-Icon korrekt
- Local LLM erkennt Response-Format korrekt
- TokenTracker: Kostenberechnung korrigiert (Preise waren Faktor 10 zu hoch)
- Projektordner: Manuell gesetzter Ordner wird korrekt übernommen

Neue Features:
- Automatisches Config-Update: Provider-Configs werden aktualisiert wenn älter als 7 Tage
- Dynamisches Laden der Model-Preise aus Provider-Configs
- Neue Module: config_updater.py, update_configs.py
</commit_message>
<xml_diff>
--- a/QCA-AID-Codebook.xlsx
+++ b/QCA-AID-Codebook.xlsx
@@ -1592,7 +1592,7 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>openai</t>
+          <t>local</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -1607,7 +1607,7 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>gpt-5-nano</t>
+          <t>qwen2.5-coder:7b</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>

</xml_diff>